<commit_message>
Update tracker.xlsx from Admin app (v1.8)
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -2712,10 +2712,8 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>$650</t>
-        </is>
+      <c r="B2" t="n">
+        <v>520</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -2729,17 +2727,15 @@
         <v>40</v>
       </c>
       <c r="F2" t="n">
-        <v>650</v>
+        <v>520</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
         <v>2</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>$385</t>
-        </is>
+      <c r="B3" t="n">
+        <v>515</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -2753,7 +2749,7 @@
         <v>10</v>
       </c>
       <c r="F3" t="n">
-        <v>385</v>
+        <v>515</v>
       </c>
     </row>
     <row r="4">
@@ -5216,7 +5212,7 @@
         <v>5</v>
       </c>
       <c r="F2" t="n">
-        <v>650</v>
+        <v>520</v>
       </c>
       <c r="G2" t="n">
         <v>40</v>
@@ -5225,10 +5221,10 @@
         <v>55</v>
       </c>
       <c r="I2" t="n">
-        <v>690</v>
+        <v>560</v>
       </c>
       <c r="J2" t="n">
-        <v>635</v>
+        <v>505</v>
       </c>
     </row>
     <row r="3">
@@ -5250,7 +5246,7 @@
         <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>385</v>
+        <v>515</v>
       </c>
       <c r="G3" t="n">
         <v>10</v>
@@ -5259,10 +5255,10 @@
         <v>55</v>
       </c>
       <c r="I3" t="n">
-        <v>395</v>
+        <v>525</v>
       </c>
       <c r="J3" t="n">
-        <v>340</v>
+        <v>470</v>
       </c>
     </row>
     <row r="4">

</xml_diff>

<commit_message>
Update tracker.xlsx from Admin app (v1.8.8)
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Players" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Series_BuyIns" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Financial_Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HighHand_Info" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -820,10 +821,8 @@
       <c r="A2" t="n">
         <v>1</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>2025-08-08</t>
-        </is>
+      <c r="B2" s="2" t="n">
+        <v>45877</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -864,10 +863,8 @@
       <c r="A4" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>2025-09-19</t>
-        </is>
+      <c r="B4" s="2" t="n">
+        <v>45919</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
@@ -887,10 +884,8 @@
       <c r="A5" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>2025-10-10</t>
-        </is>
+      <c r="B5" s="2" t="n">
+        <v>45940</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
@@ -910,10 +905,8 @@
       <c r="A6" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>2025-11-14</t>
-        </is>
+      <c r="B6" s="2" t="n">
+        <v>45975</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
@@ -933,10 +926,8 @@
       <c r="A7" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>2025-12-12</t>
-        </is>
+      <c r="B7" s="2" t="n">
+        <v>46003</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
@@ -956,10 +947,8 @@
       <c r="A8" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>2026-01-09</t>
-        </is>
+      <c r="B8" s="2" t="n">
+        <v>46031</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -979,10 +968,8 @@
       <c r="A9" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>2026-01-30</t>
-        </is>
+      <c r="B9" s="2" t="n">
+        <v>46052</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
@@ -1002,10 +989,8 @@
       <c r="A10" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>2026-02-20</t>
-        </is>
+      <c r="B10" s="2" t="n">
+        <v>46073</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
@@ -1025,10 +1010,8 @@
       <c r="A11" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>2026-03-13</t>
-        </is>
+      <c r="B11" s="2" t="n">
+        <v>46094</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
@@ -1048,10 +1031,8 @@
       <c r="A12" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>2026-04-03</t>
-        </is>
+      <c r="B12" s="2" t="n">
+        <v>46115</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
@@ -1071,10 +1052,8 @@
       <c r="A13" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>2026-04-24</t>
-        </is>
+      <c r="B13" s="2" t="n">
+        <v>46136</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1094,10 +1073,8 @@
       <c r="A14" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>2026-05-08</t>
-        </is>
+      <c r="B14" s="2" t="n">
+        <v>46150</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
@@ -6896,4 +6873,61 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Current Holder</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hand Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Display Value (override)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-08-10 14:20 UTC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update tracker.xlsx — 2025-08-10 19:23 UTC
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Players" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Series_BuyIns" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Financial_Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HighHand_Info" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6896,4 +6897,61 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Current Holder</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hand Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Display Value (override)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-08-10 19:23 UTC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update tracker.xlsx — 2025-08-10 19:24 UTC
</commit_message>
<xml_diff>
--- a/tracker.xlsx
+++ b/tracker.xlsx
@@ -14,6 +14,7 @@
     <sheet name="Players" sheetId="5" state="visible" r:id="rId5"/>
     <sheet name="Series_BuyIns" sheetId="6" state="visible" r:id="rId6"/>
     <sheet name="Financial_Summary" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HighHand_Info" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -6896,4 +6897,61 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Current Holder</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Hand Description</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Display Value (override)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Last Updated</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-08-10 19:24 UTC</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>